<commit_message>
updated remarks for rhel7.8 and rhel6 results
</commit_message>
<xml_diff>
--- a/cvmfs_test_matrix.xlsx
+++ b/cvmfs_test_matrix.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>CVMFS Test Matrix</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>only cvmfsexec works when fuse/fusermount is not available</t>
+  </si>
+  <si>
+    <t>mountrepo works even with the user not in fuse group</t>
+  </si>
+  <si>
+    <t>mountrepo requires fuse/fusermount to be available</t>
   </si>
   <si>
     <t>RHEL7.6</t>
@@ -256,6 +265,15 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -265,16 +283,7 @@
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1357,7 +1366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:H34"/>
+  <dimension ref="A2:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1424,463 +1433,489 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s" s="10">
+      <c r="B5" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s" s="13">
         <v>11</v>
       </c>
       <c r="G5" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="H5" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="H5" t="s" s="13">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H6" s="11"/>
+      <c r="A6" s="8"/>
+      <c r="B6" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s" s="13">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H7" s="11"/>
+      <c r="A7" s="8"/>
+      <c r="B7" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s" s="13">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s" s="10">
+      <c r="A8" s="8"/>
+      <c r="B8" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s" s="13">
         <v>11</v>
       </c>
       <c r="G8" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="H8" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H9" s="11"/>
+      <c r="A9" s="8"/>
+      <c r="B9" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" s="8"/>
+      <c r="B10" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="8">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="H12" s="11"/>
+      <c r="A12" t="s" s="11">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s" s="10">
-        <v>14</v>
-      </c>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H14" s="11"/>
+      <c r="A14" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H15" s="11"/>
+      <c r="A15" s="8"/>
+      <c r="B15" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s" s="13">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="H16" s="11"/>
+      <c r="A16" s="8"/>
+      <c r="B16" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="A17" s="8"/>
+      <c r="B17" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="8">
-        <v>15</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="A18" s="8"/>
+      <c r="B18" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="A20" t="s" s="11">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="12"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G20">
       <formula1>",Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated the matrix with notes and color codes
</commit_message>
<xml_diff>
--- a/cvmfs_test_matrix.xlsx
+++ b/cvmfs_test_matrix.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>CVMFS Test Matrix</t>
   </si>
@@ -34,7 +34,7 @@
     <t>mountrepo/umountrepo works?</t>
   </si>
   <si>
-    <t>Remarks</t>
+    <t>Test remarks</t>
   </si>
   <si>
     <t>RHEL8</t>
@@ -52,22 +52,55 @@
     <t>only cvmfsexec works when fuse/fusermount is not available</t>
   </si>
   <si>
-    <t>mountrepo works even with the user not in fuse group</t>
-  </si>
-  <si>
-    <t>mountrepo requires fuse/fusermount to be available</t>
-  </si>
-  <si>
-    <t>RHEL7.6</t>
-  </si>
-  <si>
-    <t>RHEL6+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fusermount becomes available only when the user is in the ‘fuse’ group </t>
+    <t>only cvmfsexec works (mountrepo requires fuse/fusermount)</t>
+  </si>
+  <si>
+    <t>mountrepo works (even though the user is not in fuse group)</t>
+  </si>
+  <si>
+    <t>mountrepo works</t>
+  </si>
+  <si>
+    <t>neither cvmfsexec nor mountrepo works (error related to unshare)</t>
+  </si>
+  <si>
+    <t>RHEL &lt;= 7.7</t>
+  </si>
+  <si>
+    <t>neither cvmfsexec nor mountrepo works (failed to exec fusermount)</t>
+  </si>
+  <si>
+    <t>(includes RHEL6)</t>
+  </si>
+  <si>
+    <t>neither cvmfsexec nor mountrepo works (permission denied error)</t>
+  </si>
+  <si>
+    <t>only cvmfsexec works since fuse/fusermount is not available</t>
+  </si>
+  <si>
+    <t>mountrepo should work (even though the user is not in fuse group)</t>
+  </si>
+  <si>
+    <t>mountrepo should work</t>
   </si>
   <si>
     <t>Non-RHEL</t>
+  </si>
+  <si>
+    <t>NOTE: using mountrepo requires umountrepo to unmount the repositories and does not clear the mount points upon exit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: In RHEL7.8, fusermount comes with fuse and does not require the user to be in fuse group </t>
+  </si>
+  <si>
+    <t>NOTE: In RHEL6+, fusermount is available only when the user is in fuse group and not with just fuse installed</t>
+  </si>
+  <si>
+    <t>NOTE: not tested with prototype</t>
+  </si>
+  <si>
+    <t>NOTE: This case assumes that fusermount is available with installation of fuse even without the user being in the fuse group (similar to RHEL7.8)</t>
   </si>
 </sst>
 </file>
@@ -95,7 +128,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +150,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -240,7 +309,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -284,6 +353,39 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -307,7 +409,13 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="fffdad00"/>
+      <rgbColor rgb="fffe634d"/>
       <rgbColor rgb="ff60d836"/>
+      <rgbColor rgb="fffff056"/>
+      <rgbColor rgb="ff72fce9"/>
+      <rgbColor rgb="ff56c1fe"/>
+      <rgbColor rgb="ffff94ca"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1366,7 +1474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:H36"/>
+  <dimension ref="A2:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1374,12 +1482,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3906" style="1" customWidth="1"/>
     <col min="2" max="3" width="20" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.2344" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.0781" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6406" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5391" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.0938" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.9062" style="1" customWidth="1"/>
     <col min="8" max="8" width="55.7969" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -1455,7 +1563,7 @@
       <c r="D5" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" t="s" s="14">
         <v>11</v>
       </c>
       <c r="F5" t="s" s="13">
@@ -1464,7 +1572,7 @@
       <c r="G5" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="H5" t="s" s="13">
+      <c r="H5" t="s" s="15">
         <v>12</v>
       </c>
     </row>
@@ -1477,18 +1585,18 @@
         <v>10</v>
       </c>
       <c r="D6" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E6" t="s" s="14">
+        <v>11</v>
       </c>
       <c r="F6" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s" s="15">
         <v>13</v>
       </c>
     </row>
@@ -1501,77 +1609,81 @@
         <v>10</v>
       </c>
       <c r="D7" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s" s="13">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E7" t="s" s="14">
+        <v>10</v>
       </c>
       <c r="F7" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s" s="17">
         <v>14</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" t="s" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s" s="13">
         <v>10</v>
       </c>
       <c r="D8" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s" s="13">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E8" t="s" s="14">
+        <v>10</v>
       </c>
       <c r="F8" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="H8" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="G8" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s" s="17">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" t="s" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E9" t="s" s="14">
+        <v>11</v>
       </c>
       <c r="F9" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="G9" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="H9" s="10"/>
+      <c r="G9" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s" s="15">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" t="s" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="E10" t="s" s="13">
+      <c r="E10" t="s" s="14">
         <v>11</v>
       </c>
       <c r="F10" t="s" s="13">
@@ -1580,29 +1692,57 @@
       <c r="G10" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="H10" s="10"/>
+      <c r="H10" t="s" s="15">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="B11" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s" s="17">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="11">
+      <c r="A12" s="8"/>
+      <c r="B12" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s" s="17">
         <v>15</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="8"/>
@@ -1616,7 +1756,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s" s="12">
         <v>11</v>
@@ -1625,21 +1765,25 @@
         <v>11</v>
       </c>
       <c r="D14" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="H14" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="G14" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s" s="15">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8"/>
+      <c r="A15" t="s" s="11">
+        <v>19</v>
+      </c>
       <c r="B15" t="s" s="12">
         <v>11</v>
       </c>
@@ -1647,19 +1791,19 @@
         <v>11</v>
       </c>
       <c r="D15" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s" s="13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="H15" t="s" s="13">
-        <v>17</v>
+      <c r="H15" t="s" s="15">
+        <v>18</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
@@ -1671,18 +1815,20 @@
         <v>11</v>
       </c>
       <c r="D16" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s" s="18">
         <v>11</v>
       </c>
       <c r="F16" t="s" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" t="s" s="15">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="8"/>
@@ -1693,122 +1839,222 @@
         <v>11</v>
       </c>
       <c r="D17" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s" s="13">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E17" t="s" s="18">
+        <v>10</v>
       </c>
       <c r="F17" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="H17" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="G17" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s" s="17">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="8"/>
-      <c r="B18" t="s" s="12">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s" s="13">
-        <v>11</v>
-      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="B19" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s" s="19">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s" s="19">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="B20" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s" s="19">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s" s="19">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="B21" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s" s="20">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s" s="19">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s" s="19">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="B22" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s" s="20">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s" s="19">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s" s="19">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="B23" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s" s="19">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s" s="19">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="B24" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s" s="19">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s" s="19">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="B25" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s" s="20">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s" s="19">
+        <v>10</v>
+      </c>
+      <c r="H25" t="s" s="19">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="B26" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s" s="20">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s" s="19">
+        <v>10</v>
+      </c>
+      <c r="H26" t="s" s="19">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" s="8"/>
@@ -1821,7 +2067,9 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="8"/>
+      <c r="A28" t="s" s="11">
+        <v>24</v>
+      </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1840,13 +2088,23 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" ht="20.05" customHeight="1">
+    <row r="30" ht="140.05" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="B30" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s" s="22">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s" s="23">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s" s="24">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s" s="25">
+        <v>29</v>
+      </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
@@ -1910,12 +2168,92 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G17 B19:G26 B28:G28">
       <formula1>",Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>